<commit_message>
Add report generator and small fixes
</commit_message>
<xml_diff>
--- a/Evaluation_Result.xlsx
+++ b/Evaluation_Result.xlsx
@@ -451,7 +451,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-10-08 16:01:39</t>
+          <t>2025-10-09 11:37:07</t>
         </is>
       </c>
     </row>
@@ -562,7 +562,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>3691</v>
+        <v>3690</v>
       </c>
     </row>
     <row r="14">
@@ -632,7 +632,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1345,7 +1345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1393,136 +1393,298 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>52060800050012</t>
+          <t>52060800020002</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>52060800050011</t>
+          <t>52060800021005</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>122400.297211675</v>
+        <v>41224.30805170261</v>
       </c>
       <c r="D2" t="n">
-        <v>270263.5685508295</v>
+        <v>42167.66026968733</v>
       </c>
       <c r="E2" t="n">
-        <v>122400.297211675</v>
+        <v>10100.23377610135</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>0.2450067509546517</v>
       </c>
       <c r="G2" t="n">
-        <v>0.4528923297653223</v>
+        <v>0.2395255916857689</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>52060800050017</t>
+          <t>52060800020003</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>52060800050016</t>
+          <t>52060800022008</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>15423.42325961922</v>
+        <v>32303.77980558742</v>
       </c>
       <c r="D3" t="n">
-        <v>2883.437007030753</v>
+        <v>145182.3518493054</v>
       </c>
       <c r="E3" t="n">
-        <v>2791.950138016949</v>
+        <v>15434.23423791282</v>
       </c>
       <c r="F3" t="n">
-        <v>0.1810201335346015</v>
+        <v>0.4777841581016237</v>
       </c>
       <c r="G3" t="n">
-        <v>0.9682715908859012</v>
+        <v>0.1063093002786802</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>52060800050018</t>
+          <t>52060800050012</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>52060800050016</t>
+          <t>52060800050011</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>7540.410064111213</v>
+        <v>122400.297211675</v>
       </c>
       <c r="D4" t="n">
-        <v>1186.639068642798</v>
+        <v>270263.5685508295</v>
       </c>
       <c r="E4" t="n">
-        <v>1186.639068642798</v>
+        <v>122400.297211675</v>
       </c>
       <c r="F4" t="n">
-        <v>0.1573706281957581</v>
+        <v>1</v>
       </c>
       <c r="G4" t="n">
-        <v>1</v>
+        <v>0.4528923297653223</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>52060800050018</t>
+          <t>52060800050017</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>52060800050015</t>
+          <t>52060800050016</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>7540.410064111213</v>
+        <v>15423.42325961922</v>
       </c>
       <c r="D5" t="n">
-        <v>0.02071007287384314</v>
+        <v>2883.437007030753</v>
       </c>
       <c r="E5" t="n">
-        <v>0.02071007287384314</v>
+        <v>2791.950138016949</v>
       </c>
       <c r="F5" t="n">
-        <v>2.746544643826905e-06</v>
+        <v>0.1810201335346015</v>
       </c>
       <c r="G5" t="n">
-        <v>1</v>
+        <v>0.9682715908859012</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>52060800050018</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>52060800050016</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>7540.410064111213</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1186.639068642798</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1186.639068642798</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.1573706281957581</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>52060800050018</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>52060800050015</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>7540.410064111213</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.02071007287384314</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.02071007287384314</v>
+      </c>
+      <c r="F7" t="n">
+        <v>2.746544643826905e-06</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>52060800050006</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>52060800051004</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>17011.19436189108</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1672752.195255189</v>
+      </c>
+      <c r="E8" t="n">
+        <v>5709.037937349282</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.3356047680072846</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.003412960959515185</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
           <t>52060800050023</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B9" t="inlineStr">
         <is>
           <t>52060800050005</t>
         </is>
       </c>
-      <c r="C6" t="n">
+      <c r="C9" t="n">
         <v>44954.81772431835</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D9" t="n">
         <v>105421.6830197758</v>
       </c>
-      <c r="E6" t="n">
+      <c r="E9" t="n">
         <v>27763.44943372393</v>
       </c>
-      <c r="F6" t="n">
+      <c r="F9" t="n">
         <v>0.6175856301760794</v>
       </c>
-      <c r="G6" t="n">
+      <c r="G9" t="n">
         <v>0.2633561582252094</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>52060800050005</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>52060800051004</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>97407.99722729861</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1672752.195255189</v>
+      </c>
+      <c r="E10" t="n">
+        <v>28268.63710708431</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.2902085856577084</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.0168994769143147</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>52060800080003</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>52060800081001</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>10663.37631213075</v>
+      </c>
+      <c r="D11" t="n">
+        <v>139176.3641311153</v>
+      </c>
+      <c r="E11" t="n">
+        <v>3128.28280175185</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.2933670078015618</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.02247711255630128</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>52060800120002</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>52060800120003</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>14675.98062515429</v>
+      </c>
+      <c r="D12" t="n">
+        <v>26449.51773102354</v>
+      </c>
+      <c r="E12" t="n">
+        <v>3853.087095435435</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.2625437573030952</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.1456770265007901</v>
       </c>
     </row>
   </sheetData>

</xml_diff>